<commit_message>
8- Added MetaViewer Login Credentials
</commit_message>
<xml_diff>
--- a/Resources/Logins.xlsx
+++ b/Resources/Logins.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="22995" windowHeight="9780"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="20580" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MetaV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>User names</t>
   </si>
@@ -32,13 +33,22 @@
   </si>
   <si>
     <t>SERVICE$08</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>ajenkins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,16 +56,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,12 +93,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,36 +464,82 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>